<commit_message>
modify in file navbar, helpers, disbursementPage, signIn & riwayatTopUp, dan add new file for template bulk disbursement
</commit_message>
<xml_diff>
--- a/src/assets/files/Template Bulk Disbursement PT. Ezeelink Indonesia.xlsx
+++ b/src/assets/files/Template Bulk Disbursement PT. Ezeelink Indonesia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ezeelink\PaymentGatewayPortalGit\PaymentGatewayPortal\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D58AA4-7067-4E7D-8821-1C4261F4502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A184B68-5156-4184-971F-DC86FCE45CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="11700" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Bulk duplikat Disburse" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Bank Tujuan*</t>
-  </si>
-  <si>
-    <t>Cabang (Khusus Non-BCA)*</t>
   </si>
   <si>
     <t>No. Rekening Tujuan*</t>
@@ -41,6 +38,9 @@
   </si>
   <si>
     <t>Catatan</t>
+  </si>
+  <si>
+    <t>Cabang*</t>
   </si>
 </sst>
 </file>
@@ -892,7 +892,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,22 +911,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>